<commit_message>
sua loi export excel
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CongViec\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CongViec\MyProjects\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADE965A-CE83-4509-A8C3-C63F97892E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C38203C-DF45-483B-8B59-FE1AAD0C663F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>HTTTTT Quản lý Đơn thư Khiếu nại, Tố cáo</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>15/03/2023 09:00</t>
+  </si>
+  <si>
+    <t>Lĩnh vực:</t>
   </si>
 </sst>
 </file>
@@ -115,8 +118,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="170" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -179,40 +182,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,156 +533,161 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.77734375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="21.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="12"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="12"/>
+        <v>15</v>
+      </c>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="N14" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <v>1</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="13">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="10">
         <v>44567.375</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="13" t="s">
+      <c r="H15" s="7"/>
+      <c r="I15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="11" t="s">
+      <c r="K15" s="7"/>
+      <c r="L15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
summary, file attachment excel api. them congkhai vao complain.
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CongViec\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC107A7-1AA3-4B68-BC35-21A253A16CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0733ACCB-C1F9-4998-9BA8-0DA1271993B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>HTTTTT Quản lý Đơn thư Khiếu nại, Tố cáo</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Lĩnh vực:</t>
+  </si>
+  <si>
+    <t>Công khai:</t>
   </si>
 </sst>
 </file>
@@ -526,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716B53E-13F1-4440-95CF-2CF41ED2ADD4}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -613,6 +616,11 @@
       </c>
       <c r="E11" s="8"/>
     </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
sửa lỗi endcoding trong bảng unit
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CongViec\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0733ACCB-C1F9-4998-9BA8-0DA1271993B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DD6961-B0DF-46C9-AC8C-9859672FD858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
   </bookViews>
@@ -529,8 +529,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716B53E-13F1-4440-95CF-2CF41ED2ADD4}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix dob user, excel, migration '20230622163435_update_indexs'
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CongViec\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CongViec\KNTC\SourceCode\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DD6961-B0DF-46C9-AC8C-9859672FD858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70F6C19-C1DE-4506-B8C0-A85C9A01C890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>HTTTTT Quản lý Đơn thư Khiếu nại, Tố cáo</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Xã/Phường:</t>
   </si>
   <si>
-    <t>tThời gian tiếp nhận:</t>
-  </si>
-  <si>
     <t>Kết quả:</t>
   </si>
   <si>
@@ -108,6 +105,15 @@
   </si>
   <si>
     <t>Công khai:</t>
+  </si>
+  <si>
+    <t>Từ khóa:</t>
+  </si>
+  <si>
+    <t>Người nộp đơn:</t>
+  </si>
+  <si>
+    <t>Thời gian tiếp nhận:</t>
   </si>
 </sst>
 </file>
@@ -527,12 +533,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716B53E-13F1-4440-95CF-2CF41ED2ADD4}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -578,120 +583,132 @@
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
       <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="8"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="8"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L14" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="N16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>1</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="9">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="9">
         <v>44567.625</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="9">
+      <c r="H17" s="7"/>
+      <c r="I17" s="9">
         <v>44567.625</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J17" s="10">
         <v>44567.375</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="10">
+      <c r="K17" s="7"/>
+      <c r="L17" s="10">
         <v>44567.375</v>
       </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update 1 loạt tính năng: 1. Hiển thị vị trí trên bản đồ 2. Cập nhật tự động zoom trên bản đồ 3. Bổ sung Sổ theo dõi đơn thư 4. Sửa lại 1 loạt báo cáo theo mẫu
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CongViec\MyProjects\HTTT_KNTC\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duong\Projects\Hau\KNTC\Code\PostgreSQL\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B97C376-2A93-428A-8CE5-45D2610B6B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B9424AD-25DA-4A23-8214-71AA833D29AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,20 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>HTTTTT Quản lý Đơn thư Khiếu nại, Tố cáo</t>
   </si>
   <si>
-    <t>DANH SÁCH ĐƠN  THƯ KHIẾU NẠI - KHIẾU KIỆN</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Đại chỉ</t>
-  </si>
-  <si>
     <t>Số ĐT</t>
   </si>
   <si>
@@ -114,17 +107,40 @@
   </si>
   <si>
     <t>Người nộp đơn</t>
+  </si>
+  <si>
+    <t>UBND tỉnh Thái Nguyên</t>
+  </si>
+  <si>
+    <t>CỘNG HÒA XÃ HỘI CHỦ NGHĨA VIỆT NAM</t>
+  </si>
+  <si>
+    <t>Sở Tài nguyên và Môi trường Thái Nguyên</t>
+  </si>
+  <si>
+    <t>Độc lập - Tự do - Hạnh phúc</t>
+  </si>
+  <si>
+    <t>---------------</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Thái Nguyên, Ngày …… Tháng ……. Năm …….</t>
+  </si>
+  <si>
+    <t>DANH SÁCH ĐƠN THƯ KHIẾU NẠI/KHIẾU KIỆN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +162,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -185,19 +214,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -207,16 +230,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -532,188 +568,231 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716B53E-13F1-4440-95CF-2CF41ED2ADD4}">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="25.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
+    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="H1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="H2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:14" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="8"/>
+        <v>9</v>
+      </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="10" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="F16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="N16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="9">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7">
         <v>44567.625</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="9">
+      <c r="H17" s="5"/>
+      <c r="I17" s="7">
         <v>44567.625</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="8">
         <v>44567.375</v>
       </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="10">
+      <c r="K17" s="5"/>
+      <c r="L17" s="8">
         <v>44567.375</v>
       </c>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="A4:N4"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bổ sung và update template Báo cáo
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$17:$N$17</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -749,43 +752,88 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="1:14" s="10" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
         <v>1</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="7">
+      <c r="B17" s="9">
+        <v>2</v>
+      </c>
+      <c r="C17" s="9">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9">
+        <v>5</v>
+      </c>
+      <c r="F17" s="9">
+        <v>6</v>
+      </c>
+      <c r="G17" s="9">
+        <v>7</v>
+      </c>
+      <c r="H17" s="9">
+        <v>8</v>
+      </c>
+      <c r="I17" s="9">
+        <v>9</v>
+      </c>
+      <c r="J17" s="9">
+        <v>10</v>
+      </c>
+      <c r="K17" s="9">
+        <v>11</v>
+      </c>
+      <c r="L17" s="9">
+        <v>12</v>
+      </c>
+      <c r="M17" s="9">
+        <v>13</v>
+      </c>
+      <c r="N17" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7">
         <v>44567.625</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="7">
+      <c r="H18" s="5"/>
+      <c r="I18" s="7">
         <v>44567.625</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J18" s="8">
         <v>44567.375</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="8">
+      <c r="K18" s="5"/>
+      <c r="L18" s="8">
         <v>44567.375</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I20" s="2" t="s">
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I21" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A17:N17"/>
   <mergeCells count="6">
     <mergeCell ref="A4:N4"/>
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Update theo cac y/c moi cua KH
</commit_message>
<xml_diff>
--- a/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/server/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -15,9 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$17:$N$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$17:$O$17</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>HTTTTT Quản lý Đơn thư Khiếu nại, Tố cáo</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Kết quả GQKN lần II</t>
   </si>
   <si>
-    <t>Kết quả</t>
-  </si>
-  <si>
     <t>Lĩnh vực:</t>
   </si>
   <si>
@@ -134,6 +131,12 @@
   </si>
   <si>
     <t>DANH SÁCH ĐƠN THƯ KHIẾU NẠI/KHIẾU KIỆN</t>
+  </si>
+  <si>
+    <t>Thẩm quyền GQKN lần I</t>
+  </si>
+  <si>
+    <t>Thẩm quyền GQKN lần II</t>
   </si>
 </sst>
 </file>
@@ -217,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,6 +249,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="A4" sqref="A4:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -590,125 +594,135 @@
     <col min="8" max="8" width="17.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.77734375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="1" customWidth="1"/>
+    <col min="11" max="12" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="18" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="11"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="H2" s="14" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H3" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="1:14" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="10" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="10" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>1</v>
       </c>
@@ -716,10 +730,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>2</v>
@@ -740,19 +754,22 @@
         <v>7</v>
       </c>
       <c r="K16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="M16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="N16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N16" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="10" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:15" s="10" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>1</v>
       </c>
@@ -795,8 +812,11 @@
       <c r="N17" s="9">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>1</v>
       </c>
@@ -816,31 +836,32 @@
         <v>44567.375</v>
       </c>
       <c r="K18" s="5"/>
-      <c r="L18" s="8">
+      <c r="L18" s="5"/>
+      <c r="M18" s="8">
         <v>44567.375</v>
       </c>
-      <c r="M18" s="5"/>
       <c r="N18" s="5"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I21" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A17:N17"/>
+  <autoFilter ref="A17:O17"/>
   <mergeCells count="6">
-    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A4:O4"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="J3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>